<commit_message>
GUI chiatique fonctionnant sauf la pratie affichage du résultat
</commit_message>
<xml_diff>
--- a/Donnees .xlsx
+++ b/Donnees .xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -509,6 +509,21 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -537,21 +552,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76937D94-5561-4F0F-AC60-CAD19876EAF5}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,11 +888,11 @@
       <c r="A1" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="70"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
@@ -1118,11 +1118,11 @@
       <c r="A23" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="43">
@@ -1156,11 +1156,11 @@
       <c r="A26" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="72"/>
-      <c r="D26" s="73"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="63"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
@@ -1386,11 +1386,11 @@
       <c r="A48" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="63" t="s">
+      <c r="B48" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C48" s="63"/>
-      <c r="D48" s="64"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="69"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
@@ -1426,23 +1426,23 @@
       <c r="A51" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="65" t="s">
+      <c r="B51" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="65"/>
-      <c r="D51" s="65"/>
+      <c r="C51" s="70"/>
+      <c r="D51" s="70"/>
       <c r="E51" s="19"/>
-      <c r="F51" s="66" t="s">
+      <c r="F51" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="G51" s="66"/>
-      <c r="H51" s="66"/>
+      <c r="G51" s="71"/>
+      <c r="H51" s="71"/>
       <c r="I51" s="19"/>
-      <c r="J51" s="67" t="s">
+      <c r="J51" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="K51" s="67"/>
-      <c r="L51" s="68"/>
+      <c r="K51" s="72"/>
+      <c r="L51" s="73"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="20"/>
@@ -1780,23 +1780,23 @@
       <c r="A65" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B65" s="59" t="s">
+      <c r="B65" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="59"/>
-      <c r="D65" s="59"/>
+      <c r="C65" s="64"/>
+      <c r="D65" s="64"/>
       <c r="E65" s="2"/>
-      <c r="F65" s="60" t="s">
+      <c r="F65" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="G65" s="60"/>
-      <c r="H65" s="60"/>
+      <c r="G65" s="65"/>
+      <c r="H65" s="65"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="61" t="s">
+      <c r="J65" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="K65" s="61"/>
-      <c r="L65" s="62"/>
+      <c r="K65" s="66"/>
+      <c r="L65" s="67"/>
     </row>
     <row r="66" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="29">
@@ -1873,16 +1873,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J65:L65"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="J51:L51"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B65:D65"/>
     <mergeCell ref="F65:H65"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="J51:L51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>